<commit_message>
Update OTW Sidang 3
</commit_message>
<xml_diff>
--- a/timeline/Data Kuesioner.xlsx
+++ b/timeline/Data Kuesioner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STMIK PRIMAKARA\SEMESTER 8\Tugas Akhir\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9007A7-48B3-49D2-BD51-AF8CED118E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0397E5E9-9D70-4BE8-8A3F-D0198F68F285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA MENTAH" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="100">
   <si>
     <t>Nama</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>Setuju</t>
+  </si>
+  <si>
+    <t>2 x 3</t>
   </si>
 </sst>
 </file>
@@ -850,7 +853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -1989,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0F242E-2242-49EC-A1BD-BC56BCC36C71}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,7 +2050,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C5" s="9">
         <f>'TOTAL RESPONDEN'!E3*3</f>
@@ -2824,11 +2827,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A80:B80"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A64:C64"/>
     <mergeCell ref="A8:B8"/>
@@ -2842,6 +2840,11 @@
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A80:B80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="168" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>